<commit_message>
final report as xlsx
</commit_message>
<xml_diff>
--- a/src/templates/final_report.xlsx
+++ b/src/templates/final_report.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11214"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Luke\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sawczak/Desktop/repos/non ics/duolingo-marker/src/templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2A0D0709-451C-41BE-8B06-D5CDBAB59F40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9B626CD-5325-C948-BEDA-C845A488852C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{8A9F5644-8153-49BB-A324-D41BED6A38CD}"/>
+    <workbookView xWindow="0" yWindow="620" windowWidth="33600" windowHeight="19160" xr2:uid="{8A9F5644-8153-49BB-A324-D41BED6A38CD}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -167,7 +167,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -486,18 +486,18 @@
   <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.90625" style="4"/>
+    <col min="1" max="1" width="28.83203125" style="4" customWidth="1"/>
     <col min="7" max="7" width="11" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.81640625" customWidth="1"/>
-    <col min="9" max="9" width="22.90625" customWidth="1"/>
+    <col min="8" max="8" width="15.83203125" customWidth="1"/>
+    <col min="9" max="9" width="22.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -526,7 +526,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>9</v>
       </c>
@@ -539,7 +539,7 @@
       <c r="H2" s="2"/>
       <c r="I2" s="2"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>10</v>
       </c>

</xml_diff>